<commit_message>
adds custom units, troubleshoots make_metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E3C57A-32ED-43A8-9206-9386D5301E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9447BCCD-44FF-4FAB-B2C6-BB1BB0435FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27090" yWindow="1710" windowWidth="21600" windowHeight="11175" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -61,9 +61,6 @@
     <t>orcid</t>
   </si>
   <si>
-    <t>creator</t>
-  </si>
-  <si>
     <t>California Department of Water Resources</t>
   </si>
   <si>
@@ -209,6 +206,27 @@
   </si>
   <si>
     <t>Primary Investigator</t>
+  </si>
+  <si>
+    <t>Speckled dace</t>
+  </si>
+  <si>
+    <t>Tule perch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steelhead trout </t>
+  </si>
+  <si>
+    <t>Steelhead trout</t>
+  </si>
+  <si>
+    <t>Ryon.Kurth@water.ca.gov </t>
+  </si>
+  <si>
+    <t>project lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feather River mini-Snorkel surveying</t>
   </si>
 </sst>
 </file>
@@ -589,6 +607,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -601,47 +622,69 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +698,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,11 +724,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
       <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -699,25 +751,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -728,50 +780,75 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A8" sqref="A8:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -785,31 +862,31 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -855,19 +932,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -889,22 +966,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -925,10 +1002,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -941,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,30 +1029,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1">
+        <v>36963</v>
+      </c>
+      <c r="G2" s="1">
+        <v>37125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds info to project metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9447BCCD-44FF-4FAB-B2C6-BB1BB0435FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A89C7C5-AF7B-4F47-BEB3-7D815CEEDB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -205,9 +205,6 @@
     <t xml:space="preserve">Ryon.Kurth@water.ca.gov </t>
   </si>
   <si>
-    <t>Primary Investigator</t>
-  </si>
-  <si>
     <t>Speckled dace</t>
   </si>
   <si>
@@ -223,10 +220,16 @@
     <t>Ryon.Kurth@water.ca.gov </t>
   </si>
   <si>
-    <t>project lead</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Feather River mini-Snorkel surveying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather river </t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>creator</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -669,22 +672,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -697,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,10 +734,10 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -751,7 +754,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,22 +836,22 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +908,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -941,7 +944,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -992,10 +995,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1008,6 +1011,11 @@
         <v>34</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1018,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,6 +1059,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>-121.63263600000001</v>
+      </c>
+      <c r="C2">
+        <v>-121.60463300000001</v>
+      </c>
+      <c r="D2">
+        <v>39.4621</v>
+      </c>
+      <c r="E2">
+        <v>39.212150000000001</v>
+      </c>
       <c r="F2" s="1">
         <v>36963</v>
       </c>

</xml_diff>

<commit_message>
revises abstract and methods and fixes typo in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A89C7C5-AF7B-4F47-BEB3-7D815CEEDB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A721D14C-5321-F249-AF20-67673CDC9224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67420" yWindow="3160" windowWidth="25080" windowHeight="15900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -82,9 +82,6 @@
     <t>fall run</t>
   </si>
   <si>
-    <t>juvenile production estimate</t>
-  </si>
-  <si>
     <t>Oncorhynchus tshawytscha</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>intellectual_rights_description</t>
   </si>
   <si>
-    <t>CCO</t>
-  </si>
-  <si>
     <t>funder_name</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>chinook</t>
   </si>
   <si>
-    <t>Mini Snorkel Data Feather River</t>
-  </si>
-  <si>
     <t>Feather Mini Snorkel Survey</t>
   </si>
   <si>
@@ -230,6 +221,12 @@
   </si>
   <si>
     <t>creator</t>
+  </si>
+  <si>
+    <t>CCBY</t>
+  </si>
+  <si>
+    <t>Distribution and habitat use of juvenile steelhead and other fishes of the lower Feather River</t>
   </si>
 </sst>
 </file>
@@ -251,6 +248,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -596,9 +594,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,9 +607,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -628,66 +626,66 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -701,12 +699,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -726,18 +724,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -754,12 +752,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -767,12 +765,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -783,15 +781,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -799,59 +797,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -865,31 +843,31 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -911,9 +889,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -933,18 +911,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -965,26 +943,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1001,19 +979,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1030,37 +1008,37 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>-121.63263600000001</v>

</xml_diff>